<commit_message>
add round 4 evidence
</commit_message>
<xml_diff>
--- a/arifintahu/evidence.xlsx
+++ b/arifintahu/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Work\s16\gon-evidence\arifintahu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2DD927-75CC-4975-8B20-8589E32974E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F0F942-74EF-4DAE-882C-DA52A6167F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="11" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,13 +38,14 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="99">
   <si>
     <t>TeamName</t>
   </si>
@@ -82,12 +83,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>S16 Research Ventures</t>
   </si>
   <si>
@@ -329,6 +324,24 @@
   </si>
   <si>
     <t>19C056C0C9709A50C90228E5971D2BA72BA51A47AFA2AACDD320FFED769E2FF4</t>
+  </si>
+  <si>
+    <t>30F1E8BDFF94DABE13A332F0FDEDF275917D88E7BB28FF30D2FABE99F707E60F</t>
+  </si>
+  <si>
+    <t>DC19205B9046CF76145C0AFB37DA1145B55669474CF80D9DC9D7C98B2EA4A7E1</t>
+  </si>
+  <si>
+    <t>6174EB9A4FE8F41A1E0C75DBD1EA93F28B70E34E9C867C90853F258A0C6B8915</t>
+  </si>
+  <si>
+    <t>E2E418A326380E19CCAAFB8386F359AEDBFD073148EAFA69A24177D2C4770D2B</t>
+  </si>
+  <si>
+    <t>7E0B27634F6E45F4D25C63F898E27B3D41F25137EA384A3EE68B794676114062</t>
+  </si>
+  <si>
+    <t>7E21D3EEA04ABD3A98E30DD2FC846C65BB3DDAF201D7E8657B55D77243FD6759</t>
   </si>
 </sst>
 </file>
@@ -806,28 +819,28 @@
     </row>
     <row r="2" spans="1:8" ht="13.8">
       <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -859,10 +872,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -894,10 +907,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -929,10 +942,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -964,10 +977,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -980,7 +993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -999,34 +1012,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.8">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1058,34 +1071,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.8">
       <c r="A5" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1117,34 +1130,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.8">
       <c r="A5" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1176,34 +1189,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.8">
       <c r="A5" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1235,34 +1248,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.8">
       <c r="A5" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1295,34 +1308,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.8">
       <c r="A5" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1354,10 +1367,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1389,50 +1402,50 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="13.8">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13.8">
       <c r="A7" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1464,50 +1477,50 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1533,12 +1546,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1568,12 +1581,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1591,7 +1604,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -1603,12 +1616,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1625,9 +1638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
   <sheetData>
@@ -1638,12 +1649,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.8">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1653,6 +1664,37 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89A689E-B104-4313-81C7-88CE7F99957F}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="13.8">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="13.8">
+      <c r="A2" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="13.8">
+      <c r="A3" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1683,46 +1725,46 @@
     </row>
     <row r="2" spans="1:3" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.8">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.8">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.8">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1762,16 +1804,16 @@
     </row>
     <row r="2" spans="1:7" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1812,16 +1854,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1860,16 +1902,16 @@
     </row>
     <row r="2" spans="1:7" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1912,16 +1954,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.8">
       <c r="A2" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1953,10 +1995,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1988,10 +2030,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>